<commit_message>
Excel Data Reader Working
</commit_message>
<xml_diff>
--- a/Mars_Competition_Task/Spreadsheets/Share Skill.xlsx
+++ b/Mars_Competition_Task/Spreadsheets/Share Skill.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankur\Desktop\Mars_Competition_Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankur\Desktop\Mars_Competition_Task\Mars_Competition_Task\Mars_Competition_Task\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91751DB-8F12-4AD9-B786-6D75A2C0C18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AA3405-6B6D-4612-B258-D0415679C5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ShareSkill" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Description</t>
   </si>
@@ -34,25 +34,7 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>Service Type</t>
-  </si>
-  <si>
-    <t>Location Type</t>
-  </si>
-  <si>
-    <t>Skill Trade</t>
-  </si>
-  <si>
-    <t>Skill-Exchange</t>
-  </si>
-  <si>
     <t>Work Samples</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
   <si>
     <t>Ankur Singhal</t>
@@ -72,22 +54,22 @@
     <t>On-site</t>
   </si>
   <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t>End date (optional)</t>
-  </si>
-  <si>
     <t>Credit</t>
   </si>
   <si>
     <t>Share Skill.xlsx</t>
   </si>
   <si>
-    <t>Hidden</t>
-  </si>
-  <si>
     <t>https://www.add-in-express.com/forum/read.php?FID=5&amp;TID=15525</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Tag</t>
   </si>
 </sst>
 </file>
@@ -145,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -156,7 +138,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -439,31 +420,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -472,69 +448,44 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>